<commit_message>
Update model and adds new samples
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample90-file-headerinfo.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample90-file-headerinfo.xlsx
@@ -5,12 +5,12 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="EPPlus - Some data" sheetId="1" r:id="rId1"/>
+    <sheet name="EPPlus - Some data with header" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EPPlus - Some data'!$B$5:$F$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'EPPlus - Some data'!$A$1:$F$12</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'EPPlus - Some data'!$1:$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EPPlus - Some data with header'!$B$5:$F$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'EPPlus - Some data with header'!$A$1:$F$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'EPPlus - Some data with header'!$1:$5</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>